<commit_message>
modification tableau + ajout image stage
</commit_message>
<xml_diff>
--- a/Ressources/Annexe 6-1 - Tableau de synthèse - Épreuve E4 - BTS SIO 2022.xlsx
+++ b/Ressources/Annexe 6-1 - Tableau de synthèse - Épreuve E4 - BTS SIO 2022.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\portfolio\Ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E954495-AD32-4951-A983-C88299FC6B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB54814C-8785-4819-A1FF-686793F87B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11568" yWindow="1044" windowWidth="11472" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$19</definedName>
   </definedNames>
   <calcPr calcId="101716"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -164,7 +164,16 @@
     <t>25/05/2021-25/06/2021</t>
   </si>
   <si>
-    <t>03/01/2022-04/02/2022</t>
+    <t>03/01/2022-19/01/2022</t>
+  </si>
+  <si>
+    <t>20/01/2022-04/02/2022</t>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
   </si>
 </sst>
 </file>
@@ -245,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -460,12 +469,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -521,6 +556,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,6 +584,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -905,10 +952,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ64"/>
+  <dimension ref="A1:AQ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -921,56 +968,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="19"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="20" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -982,10 +1029,10 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1008,8 +1055,8 @@
       </c>
     </row>
     <row r="6" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="18" t="s">
         <v>9</v>
       </c>
@@ -1065,16 +1112,16 @@
       <c r="AQ6"/>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -1122,9 +1169,7 @@
       <c r="D8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>30</v>
-      </c>
+      <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="17"/>
@@ -1175,9 +1220,7 @@
       <c r="D9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>30</v>
-      </c>
+      <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="17"/>
@@ -1268,7 +1311,7 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
@@ -1283,9 +1326,7 @@
       <c r="F11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>30</v>
-      </c>
+      <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -1323,25 +1364,23 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>30</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="16"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1378,17 +1417,23 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1425,23 +1470,17 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17"/>
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1478,17 +1517,23 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1525,31 +1570,17 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>30</v>
-      </c>
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1588,20 +1619,14 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>30</v>
-      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1647,15 +1672,25 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1692,7 +1727,51 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AN19"/>
+      <c r="AO19"/>
+      <c r="AP19"/>
+      <c r="AQ19"/>
+    </row>
     <row r="20" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1738,13 +1817,14 @@
     <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A16:H16"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>

</xml_diff>